<commit_message>
Complete EVAL section analysis code
</commit_message>
<xml_diff>
--- a/A_Input/twitter_handles.xlsx
+++ b/A_Input/twitter_handles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/word_choice_communities/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79B7D82-4658-694C-A83E-E3C2BD0F67BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244143AE-3E33-1E43-BE71-80DF748E1F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1820" windowWidth="17300" windowHeight="21100" xr2:uid="{BCB6CF97-4FB3-B941-833D-11AB9E201DC0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4006" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4006" uniqueCount="1722">
   <si>
     <t>group</t>
   </si>
@@ -5197,6 +5197,9 @@
   </si>
   <si>
     <t>https://twitter.com/rechievaldez</t>
+  </si>
+  <si>
+    <t>https://twitter.com/stenyhoyer</t>
   </si>
 </sst>
 </file>
@@ -5653,8 +5656,8 @@
   <dimension ref="A1:J797"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8990,7 +8993,7 @@
         <v>477</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>1098</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Begin generating statistics and figures for pptx
</commit_message>
<xml_diff>
--- a/A_Input/twitter_handles.xlsx
+++ b/A_Input/twitter_handles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s8/Documents/Coding/word_choice_communities/A_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244143AE-3E33-1E43-BE71-80DF748E1F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800BED96-52DE-C447-8642-CD07595C36D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1820" windowWidth="17300" windowHeight="21100" xr2:uid="{BCB6CF97-4FB3-B941-833D-11AB9E201DC0}"/>
+    <workbookView xWindow="11140" yWindow="500" windowWidth="17300" windowHeight="21100" xr2:uid="{BCB6CF97-4FB3-B941-833D-11AB9E201DC0}"/>
   </bookViews>
   <sheets>
     <sheet name="handles" sheetId="1" r:id="rId1"/>
@@ -5656,7 +5656,7 @@
   <dimension ref="A1:J797"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A768" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
@@ -19394,7 +19394,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19468,21 +19468,21 @@
       <c r="B7" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>1708</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>600</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>